<commit_message>
classification and the result
</commit_message>
<xml_diff>
--- a/result/orig_classfication_classifiers_result.xlsx
+++ b/result/orig_classfication_classifiers_result.xlsx
@@ -670,88 +670,88 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5580807645890563</v>
+        <v>0.6015231667975562</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5700000000000001</v>
+        <v>0.6220000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5504950905268109</v>
+        <v>0.5914127684875644</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5509999999999999</v>
+        <v>0.5965</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6056530672714828</v>
+        <v>0.63333111688227</v>
       </c>
       <c r="G4" t="n">
-        <v>0.623</v>
+        <v>0.656</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5947672303014579</v>
+        <v>0.6165133457027109</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5915</v>
+        <v>0.6185</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5133491337347751</v>
+        <v>0.5111399538790977</v>
       </c>
       <c r="K4" t="n">
-        <v>0.511</v>
+        <v>0.513</v>
       </c>
       <c r="L4" t="n">
-        <v>0.523151499444</v>
+        <v>0.5150948030852934</v>
       </c>
       <c r="M4" t="n">
-        <v>0.522</v>
+        <v>0.5165</v>
       </c>
       <c r="N4" t="n">
-        <v>0.6037497837358261</v>
+        <v>0.6308840169499776</v>
       </c>
       <c r="O4" t="n">
-        <v>0.6359999999999999</v>
+        <v>0.6609999999999999</v>
       </c>
       <c r="P4" t="n">
-        <v>0.5811938297220145</v>
+        <v>0.6119448440155988</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.584</v>
+        <v>0.6144999999999999</v>
       </c>
       <c r="R4" t="n">
-        <v>0.5686677740467572</v>
+        <v>0.6032757859987367</v>
       </c>
       <c r="S4" t="n">
-        <v>0.6020000000000001</v>
+        <v>0.619</v>
       </c>
       <c r="T4" t="n">
-        <v>0.544831610843776</v>
+        <v>0.5978477645633143</v>
       </c>
       <c r="U4" t="n">
-        <v>0.5485</v>
+        <v>0.601</v>
       </c>
       <c r="V4" t="n">
-        <v>0.6070424555767905</v>
+        <v>0.6270932346735956</v>
       </c>
       <c r="W4" t="n">
-        <v>0.6270000000000001</v>
+        <v>0.649</v>
       </c>
       <c r="X4" t="n">
-        <v>0.5932317750128624</v>
+        <v>0.6111703256818759</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.591</v>
+        <v>0.6135</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.6037624577960379</v>
+        <v>0.632592589492169</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.6359999999999999</v>
+        <v>0.662</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.5813202974911583</v>
+        <v>0.6150457195910861</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.583</v>
+        <v>0.6165</v>
       </c>
     </row>
     <row r="5">
@@ -761,88 +761,88 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.524114423166566</v>
+        <v>0.6522627909298521</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5229999999999999</v>
+        <v>0.842</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5410112368800885</v>
+        <v>0.5340715536244627</v>
       </c>
       <c r="E5" t="n">
-        <v>0.537</v>
+        <v>0.554</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6787574469993511</v>
+        <v>0.6643208308976678</v>
       </c>
       <c r="G5" t="n">
-        <v>0.89</v>
+        <v>0.8530000000000001</v>
       </c>
       <c r="H5" t="n">
-        <v>0.552784846336431</v>
+        <v>0.5499871638906561</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5785</v>
+        <v>0.573</v>
       </c>
       <c r="J5" t="n">
-        <v>0.677460317875371</v>
+        <v>0.6745290942310661</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9620000000000001</v>
+        <v>0.969</v>
       </c>
       <c r="L5" t="n">
-        <v>0.523779124346939</v>
+        <v>0.5178499292574488</v>
       </c>
       <c r="M5" t="n">
-        <v>0.542</v>
+        <v>0.5325</v>
       </c>
       <c r="N5" t="n">
-        <v>0.6723085426783755</v>
+        <v>0.6629241030651151</v>
       </c>
       <c r="O5" t="n">
-        <v>0.852</v>
+        <v>0.85</v>
       </c>
       <c r="P5" t="n">
-        <v>0.5604079630010261</v>
+        <v>0.5466654128797196</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.586</v>
+        <v>0.57</v>
       </c>
       <c r="R5" t="n">
-        <v>0.6754820565278064</v>
+        <v>0.6621633841833641</v>
       </c>
       <c r="S5" t="n">
-        <v>0.9429999999999999</v>
+        <v>0.8779999999999999</v>
       </c>
       <c r="T5" t="n">
-        <v>0.527806533683791</v>
+        <v>0.5328773928810653</v>
       </c>
       <c r="U5" t="n">
-        <v>0.5485</v>
+        <v>0.5535</v>
       </c>
       <c r="V5" t="n">
-        <v>0.6813897801337265</v>
+        <v>0.6752951959547212</v>
       </c>
       <c r="W5" t="n">
-        <v>0.9299999999999999</v>
+        <v>0.9229999999999998</v>
       </c>
       <c r="X5" t="n">
-        <v>0.5406656644619103</v>
+        <v>0.5347058109081386</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.5655</v>
+        <v>0.5574999999999999</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.6840860501776619</v>
+        <v>0.6645414853783831</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.925</v>
+        <v>0.875</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.5458035099765424</v>
+        <v>0.5378070532789861</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.5730000000000001</v>
+        <v>0.5599999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -852,88 +852,88 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5517188023189259</v>
+        <v>0.5745815448526939</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5389999999999999</v>
+        <v>0.5660000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5714338281394167</v>
+        <v>0.5998115209111613</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5635</v>
+        <v>0.598</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6587379374372226</v>
+        <v>0.674261384613661</v>
       </c>
       <c r="G6" t="n">
-        <v>0.678</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6636699968883695</v>
+        <v>0.6771920063597272</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6555000000000001</v>
+        <v>0.667</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5437278349357643</v>
+        <v>0.5308052570546892</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5410000000000001</v>
+        <v>0.525</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5550189713316477</v>
+        <v>0.5454438940749439</v>
       </c>
       <c r="M6" t="n">
-        <v>0.5539999999999999</v>
+        <v>0.542</v>
       </c>
       <c r="N6" t="n">
-        <v>0.6496712997319191</v>
+        <v>0.6542885348579179</v>
       </c>
       <c r="O6" t="n">
-        <v>0.665</v>
+        <v>0.6450000000000001</v>
       </c>
       <c r="P6" t="n">
-        <v>0.6627083073692643</v>
+        <v>0.6858325444875175</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.65</v>
+        <v>0.6685</v>
       </c>
       <c r="R6" t="n">
-        <v>0.5741714195354702</v>
+        <v>0.5886385471989254</v>
       </c>
       <c r="S6" t="n">
-        <v>0.572</v>
+        <v>0.5830000000000001</v>
       </c>
       <c r="T6" t="n">
-        <v>0.587285691361503</v>
+        <v>0.6142079792501705</v>
       </c>
       <c r="U6" t="n">
-        <v>0.579</v>
+        <v>0.6114999999999999</v>
       </c>
       <c r="V6" t="n">
-        <v>0.6614435664788714</v>
+        <v>0.6735301340586225</v>
       </c>
       <c r="W6" t="n">
-        <v>0.6869999999999999</v>
+        <v>0.6970000000000001</v>
       </c>
       <c r="X6" t="n">
-        <v>0.6612695812440983</v>
+        <v>0.6759493284307114</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.6545000000000001</v>
+        <v>0.663</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.6451158755277351</v>
+        <v>0.647515729959139</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.656</v>
+        <v>0.64</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.6645516308302791</v>
+        <v>0.6765137304929113</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.6465</v>
+        <v>0.6585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lbp glcm color histogram humoment feature
</commit_message>
<xml_diff>
--- a/result/orig_classfication_classifiers_result.xlsx
+++ b/result/orig_classfication_classifiers_result.xlsx
@@ -670,88 +670,88 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6015231667975562</v>
+        <v>0.5845681264288881</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6220000000000001</v>
+        <v>0.601</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5914127684875644</v>
+        <v>0.5729440557234217</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5965</v>
+        <v>0.5780000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>0.63333111688227</v>
+        <v>0.5717826952400543</v>
       </c>
       <c r="G4" t="n">
-        <v>0.656</v>
+        <v>0.572</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6165133457027109</v>
+        <v>0.576880256254212</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6185</v>
+        <v>0.575</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5111399538790977</v>
+        <v>0.5133491337347751</v>
       </c>
       <c r="K4" t="n">
-        <v>0.513</v>
+        <v>0.511</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5150948030852934</v>
+        <v>0.523151499444</v>
       </c>
       <c r="M4" t="n">
-        <v>0.5165</v>
+        <v>0.522</v>
       </c>
       <c r="N4" t="n">
-        <v>0.6308840169499776</v>
+        <v>0.6036753743931195</v>
       </c>
       <c r="O4" t="n">
-        <v>0.6609999999999999</v>
+        <v>0.6159999999999999</v>
       </c>
       <c r="P4" t="n">
-        <v>0.6119448440155988</v>
+        <v>0.6028518898370733</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.6144999999999999</v>
+        <v>0.599</v>
       </c>
       <c r="R4" t="n">
-        <v>0.6032757859987367</v>
+        <v>0.5785652225833577</v>
       </c>
       <c r="S4" t="n">
-        <v>0.619</v>
+        <v>0.59</v>
       </c>
       <c r="T4" t="n">
-        <v>0.5978477645633143</v>
+        <v>0.5729014797117272</v>
       </c>
       <c r="U4" t="n">
-        <v>0.601</v>
+        <v>0.5770000000000001</v>
       </c>
       <c r="V4" t="n">
-        <v>0.6270932346735956</v>
+        <v>0.567879956246941</v>
       </c>
       <c r="W4" t="n">
-        <v>0.649</v>
+        <v>0.5670000000000001</v>
       </c>
       <c r="X4" t="n">
-        <v>0.6111703256818759</v>
+        <v>0.5744155766747584</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.6135</v>
+        <v>0.5725</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.632592589492169</v>
+        <v>0.6034130210693378</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.662</v>
+        <v>0.615</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.6150457195910861</v>
+        <v>0.6028699011759008</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.6165</v>
+        <v>0.599</v>
       </c>
     </row>
     <row r="5">
@@ -761,88 +761,88 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6522627909298521</v>
+        <v>0.6548313376184899</v>
       </c>
       <c r="C5" t="n">
-        <v>0.842</v>
+        <v>0.835</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5340715536244627</v>
+        <v>0.5404544515196925</v>
       </c>
       <c r="E5" t="n">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.4835430185074124</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.5279999999999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.5581453462618027</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.5325</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.677460317875371</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9620000000000001</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.523779124346939</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.542</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.5238951285472165</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.585</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.5653831561873679</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.5499999999999999</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.6613780097729983</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.8700000000000001</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.5350181940300203</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.5565</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.5085330649152446</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.5659999999999999</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.5662291051619348</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.5445</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.5418062130768486</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.615</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.5656486288646392</v>
+      </c>
+      <c r="AC5" t="n">
         <v>0.554</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.6643208308976678</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.8530000000000001</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.5499871638906561</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.573</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.6745290942310661</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.969</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.5178499292574488</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.5325</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.6629241030651151</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.5466654128797196</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.6621633841833641</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.8779999999999999</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.5328773928810653</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.5535</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.6752951959547212</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.9229999999999998</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0.5347058109081386</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.5574999999999999</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0.6645414853783831</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.5378070532789861</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0.5599999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -852,88 +852,88 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5745815448526939</v>
+        <v>0.5881671239646633</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5660000000000001</v>
+        <v>0.574</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5998115209111613</v>
+        <v>0.6217608926845342</v>
       </c>
       <c r="E6" t="n">
-        <v>0.598</v>
+        <v>0.6125</v>
       </c>
       <c r="F6" t="n">
-        <v>0.674261384613661</v>
+        <v>0.6805563181047538</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.669</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6771920063597272</v>
+        <v>0.7131871496881104</v>
       </c>
       <c r="I6" t="n">
-        <v>0.667</v>
+        <v>0.6930000000000001</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5308052570546892</v>
+        <v>0.543696350475867</v>
       </c>
       <c r="K6" t="n">
-        <v>0.525</v>
+        <v>0.541</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5454438940749439</v>
+        <v>0.5553221257548028</v>
       </c>
       <c r="M6" t="n">
-        <v>0.542</v>
+        <v>0.5525</v>
       </c>
       <c r="N6" t="n">
-        <v>0.6542885348579179</v>
+        <v>0.6975852276227466</v>
       </c>
       <c r="O6" t="n">
-        <v>0.6450000000000001</v>
+        <v>0.6849999999999999</v>
       </c>
       <c r="P6" t="n">
-        <v>0.6858325444875175</v>
+        <v>0.7284479389363702</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.6685</v>
+        <v>0.7125000000000001</v>
       </c>
       <c r="R6" t="n">
-        <v>0.5886385471989254</v>
+        <v>0.589092567594468</v>
       </c>
       <c r="S6" t="n">
-        <v>0.5830000000000001</v>
+        <v>0.5740000000000001</v>
       </c>
       <c r="T6" t="n">
-        <v>0.6142079792501705</v>
+        <v>0.6209315849744621</v>
       </c>
       <c r="U6" t="n">
-        <v>0.6114999999999999</v>
+        <v>0.6129999999999999</v>
       </c>
       <c r="V6" t="n">
-        <v>0.6735301340586225</v>
+        <v>0.6871353930080181</v>
       </c>
       <c r="W6" t="n">
-        <v>0.6970000000000001</v>
+        <v>0.6679999999999999</v>
       </c>
       <c r="X6" t="n">
-        <v>0.6759493284307114</v>
+        <v>0.7272190730520369</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.663</v>
+        <v>0.7050000000000001</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.647515729959139</v>
+        <v>0.7018982612123865</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.64</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.6765137304929113</v>
+        <v>0.7403448515741375</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.6585</v>
+        <v>0.721</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature extraction using resnet and classification result
</commit_message>
<xml_diff>
--- a/result/orig_classfication_classifiers_result.xlsx
+++ b/result/orig_classfication_classifiers_result.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,60 +465,12 @@
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>texture</t>
+          <t>resnet</t>
         </is>
       </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>color</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>shape</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="n"/>
-      <c r="L1" s="1" t="n"/>
-      <c r="M1" s="1" t="n"/>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>texture-color</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="n"/>
-      <c r="P1" s="1" t="n"/>
-      <c r="Q1" s="1" t="n"/>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>texture-shape</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="n"/>
-      <c r="T1" s="1" t="n"/>
-      <c r="U1" s="1" t="n"/>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>color-shape</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="n"/>
-      <c r="X1" s="1" t="n"/>
-      <c r="Y1" s="1" t="n"/>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>texture-color-shape</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="n"/>
-      <c r="AB1" s="1" t="n"/>
-      <c r="AC1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -542,126 +494,6 @@
           <t>accuracy</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>f1</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>recall</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>precision</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>f1</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>recall</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>precision</t>
-        </is>
-      </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>f1</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>recall</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>precision</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
-      <c r="R2" s="1" t="inlineStr">
-        <is>
-          <t>f1</t>
-        </is>
-      </c>
-      <c r="S2" s="1" t="inlineStr">
-        <is>
-          <t>recall</t>
-        </is>
-      </c>
-      <c r="T2" s="1" t="inlineStr">
-        <is>
-          <t>precision</t>
-        </is>
-      </c>
-      <c r="U2" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
-      <c r="V2" s="1" t="inlineStr">
-        <is>
-          <t>f1</t>
-        </is>
-      </c>
-      <c r="W2" s="1" t="inlineStr">
-        <is>
-          <t>recall</t>
-        </is>
-      </c>
-      <c r="X2" s="1" t="inlineStr">
-        <is>
-          <t>precision</t>
-        </is>
-      </c>
-      <c r="Y2" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
-      <c r="Z2" s="1" t="inlineStr">
-        <is>
-          <t>f1</t>
-        </is>
-      </c>
-      <c r="AA2" s="1" t="inlineStr">
-        <is>
-          <t>recall</t>
-        </is>
-      </c>
-      <c r="AB2" s="1" t="inlineStr">
-        <is>
-          <t>precision</t>
-        </is>
-      </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -670,88 +502,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5845681264288881</v>
+        <v>0.7172473939986204</v>
       </c>
       <c r="C4" t="n">
-        <v>0.601</v>
+        <v>0.882</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5729440557234217</v>
+        <v>0.6134103436889233</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5780000000000001</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.5717826952400543</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.572</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.576880256254212</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.575</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.5133491337347751</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.511</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.523151499444</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.522</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.6036753743931195</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.6159999999999999</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.6028518898370733</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.599</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.5785652225833577</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.5729014797117272</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.5770000000000001</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.567879956246941</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0.5670000000000001</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0.5744155766747584</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.5725</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0.6034130210693378</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>0.615</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.6028699011759008</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>0.599</v>
+        <v>0.6499999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -761,88 +521,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6548313376184899</v>
+        <v>0.5931661476721944</v>
       </c>
       <c r="C5" t="n">
-        <v>0.835</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5404544515196925</v>
+        <v>0.6429072255320161</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5620000000000001</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.4835430185074124</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.5279999999999999</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.5581453462618027</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.5325</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.677460317875371</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.9620000000000001</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.523779124346939</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.542</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.5238951285472165</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.585</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.5653831561873679</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.5499999999999999</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.6613780097729983</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.8700000000000001</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.5350181940300203</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.5565</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.5085330649152446</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.5659999999999999</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0.5662291051619348</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.5445</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0.5418062130768486</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0.615</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.5656486288646392</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0.554</v>
+        <v>0.631</v>
       </c>
     </row>
     <row r="6">
@@ -852,99 +540,21 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5881671239646633</v>
+        <v>0.7423604957983188</v>
       </c>
       <c r="C6" t="n">
-        <v>0.574</v>
+        <v>0.76</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6217608926845342</v>
+        <v>0.7497219489911615</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6125</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.6805563181047538</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.669</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.7131871496881104</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.6930000000000001</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.543696350475867</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.541</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.5553221257548028</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.5525</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.6975852276227466</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.6849999999999999</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.7284479389363702</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.7125000000000001</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.589092567594468</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.5740000000000001</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.6209315849744621</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.6129999999999999</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.6871353930080181</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.6679999999999999</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0.7272190730520369</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0.7050000000000001</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0.7018982612123865</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0.6840000000000001</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0.7403448515741375</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0.721</v>
+        <v>0.7415</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>